<commit_message>
Añadido resultados, añadido notas de resultados, cambiada output de validacion
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/Resultados buenos/dataFrame - 70001256.xlsx
+++ b/AI_Engine/Resultados/Resultados buenos/dataFrame - 70001256.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Resultados\Resultados buenos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647DB16-6F5B-46A7-A10F-E990CB03CE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A982D9E6-E351-413F-B322-4FC1A6682050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15570" yWindow="3480" windowWidth="11325" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="116">
   <si>
     <t>archivo</t>
   </si>
@@ -220,27 +220,18 @@
     <t>360.0000</t>
   </si>
   <si>
-    <t>I12207</t>
-  </si>
-  <si>
     <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\ESP\t192.pdf</t>
   </si>
   <si>
     <t>1220684</t>
   </si>
   <si>
-    <t>RS26019</t>
-  </si>
-  <si>
     <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\ESP\t193.pdf</t>
   </si>
   <si>
     <t>1220682</t>
   </si>
   <si>
-    <t>RS20857</t>
-  </si>
-  <si>
     <t>4.0000</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>308.0000</t>
   </si>
   <si>
-    <t>Rt30367</t>
-  </si>
-  <si>
     <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\ESP\t23.pdf</t>
   </si>
   <si>
@@ -373,26 +361,47 @@
     <t>05/18/2022</t>
   </si>
   <si>
-    <t>Fecha y referencia</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
     <t>Order number</t>
+  </si>
+  <si>
+    <t>UNDER 1000#UPS COLLECT#530-7760V 1000# YELLOW FRT COLLECT</t>
+  </si>
+  <si>
+    <t>er &gt;&lt; OO,</t>
+  </si>
+  <si>
+    <t>mp</t>
+  </si>
+  <si>
+    <t>———</t>
+  </si>
+  <si>
+    <t>Shipping f</t>
+  </si>
+  <si>
+    <t>Revision Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -435,13 +444,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,23 +757,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J107"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -786,11 +798,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -803,8 +815,17 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
       <c r="I2">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -830,13 +851,13 @@
         <v>13</v>
       </c>
       <c r="I3">
-        <v>56.646999999999998</v>
+        <v>90.078000000000003</v>
       </c>
       <c r="J3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -849,8 +870,17 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
       <c r="I4">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -879,7 +909,7 @@
         <v>89.043999999999997</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -905,13 +935,13 @@
         <v>21</v>
       </c>
       <c r="I6">
-        <v>86.134</v>
+        <v>91.444000000000003</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -924,8 +954,17 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" t="s">
+        <v>114</v>
+      </c>
       <c r="I7">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -951,13 +990,13 @@
         <v>24</v>
       </c>
       <c r="I8">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -970,8 +1009,17 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" t="s">
+        <v>114</v>
+      </c>
       <c r="I9">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -997,13 +1045,13 @@
         <v>29</v>
       </c>
       <c r="I10">
-        <v>57.228000000000002</v>
+        <v>92.156999999999996</v>
       </c>
       <c r="J10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1016,8 +1064,17 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
       <c r="I11">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1043,13 +1100,13 @@
         <v>13</v>
       </c>
       <c r="I12">
-        <v>56.646999999999998</v>
+        <v>90.078000000000003</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1062,8 +1119,17 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
+      <c r="E13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
       <c r="I13">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1089,13 +1155,13 @@
         <v>18</v>
       </c>
       <c r="I14">
-        <v>85.953000000000003</v>
+        <v>90.813000000000002</v>
       </c>
       <c r="J14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1108,8 +1174,17 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
+      <c r="E15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
       <c r="I15">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1135,13 +1210,13 @@
         <v>24</v>
       </c>
       <c r="I16">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1154,8 +1229,17 @@
       <c r="D17" t="s">
         <v>10</v>
       </c>
+      <c r="E17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
       <c r="I17">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1181,13 +1265,13 @@
         <v>36</v>
       </c>
       <c r="I18">
-        <v>85.953000000000003</v>
+        <v>90.813000000000002</v>
       </c>
       <c r="J18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1200,8 +1284,17 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>114</v>
+      </c>
       <c r="I19">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1227,13 +1320,13 @@
         <v>39</v>
       </c>
       <c r="I20">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1246,8 +1339,17 @@
       <c r="D21" t="s">
         <v>10</v>
       </c>
+      <c r="E21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>114</v>
+      </c>
       <c r="I21">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1273,13 +1375,13 @@
         <v>36</v>
       </c>
       <c r="I22">
-        <v>73.58</v>
+        <v>84.751999999999995</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1292,8 +1394,17 @@
       <c r="D23" t="s">
         <v>10</v>
       </c>
+      <c r="E23" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
       <c r="I23">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1322,7 +1433,7 @@
         <v>67.394999999999996</v>
       </c>
       <c r="J24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,13 +1459,13 @@
         <v>39</v>
       </c>
       <c r="I25">
-        <v>86.134</v>
+        <v>91.444000000000003</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1367,8 +1478,17 @@
       <c r="D26" t="s">
         <v>10</v>
       </c>
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
       <c r="I26">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1394,13 +1514,13 @@
         <v>36</v>
       </c>
       <c r="I27">
-        <v>85.953000000000003</v>
+        <v>90.813000000000002</v>
       </c>
       <c r="J27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1413,8 +1533,17 @@
       <c r="D28" t="s">
         <v>10</v>
       </c>
+      <c r="E28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" t="s">
+        <v>114</v>
+      </c>
       <c r="I28">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1440,13 +1569,13 @@
         <v>52</v>
       </c>
       <c r="I29">
-        <v>57.228000000000002</v>
+        <v>84.942999999999998</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1460,10 +1589,10 @@
         <v>10</v>
       </c>
       <c r="I30">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1482,14 +1611,17 @@
       <c r="F31" t="s">
         <v>56</v>
       </c>
+      <c r="G31" t="s">
+        <v>115</v>
+      </c>
       <c r="I31">
         <v>-100</v>
       </c>
       <c r="J31" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1508,14 +1640,17 @@
       <c r="F32" t="s">
         <v>56</v>
       </c>
+      <c r="G32" t="s">
+        <v>115</v>
+      </c>
       <c r="I32">
         <v>-100</v>
       </c>
       <c r="J32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1534,14 +1669,17 @@
       <c r="F33" t="s">
         <v>56</v>
       </c>
+      <c r="G33" t="s">
+        <v>115</v>
+      </c>
       <c r="I33">
         <v>-100</v>
       </c>
       <c r="J33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1555,10 +1693,10 @@
         <v>10</v>
       </c>
       <c r="I34">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1577,14 +1715,17 @@
       <c r="F35" t="s">
         <v>60</v>
       </c>
+      <c r="G35" t="s">
+        <v>115</v>
+      </c>
       <c r="I35">
         <v>-100</v>
       </c>
       <c r="J35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1603,14 +1744,17 @@
       <c r="F36" t="s">
         <v>60</v>
       </c>
+      <c r="G36" t="s">
+        <v>115</v>
+      </c>
       <c r="I36">
         <v>-100</v>
       </c>
       <c r="J36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1629,14 +1773,17 @@
       <c r="F37" t="s">
         <v>60</v>
       </c>
+      <c r="G37" t="s">
+        <v>115</v>
+      </c>
       <c r="I37">
         <v>-100</v>
       </c>
       <c r="J37" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1650,70 +1797,76 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F38" t="s">
         <v>60</v>
       </c>
+      <c r="G38" t="s">
+        <v>115</v>
+      </c>
       <c r="I38">
         <v>-100</v>
       </c>
       <c r="J38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
         <v>62</v>
       </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
       <c r="I39">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" t="s">
         <v>62</v>
       </c>
-      <c r="C40" t="s">
-        <v>63</v>
-      </c>
       <c r="D40" t="s">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
       </c>
+      <c r="G40" t="s">
+        <v>115</v>
+      </c>
       <c r="I40">
         <v>-100</v>
       </c>
       <c r="J40" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" t="s">
         <v>62</v>
-      </c>
-      <c r="C41" t="s">
-        <v>63</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
@@ -1724,22 +1877,25 @@
       <c r="F41" t="s">
         <v>12</v>
       </c>
+      <c r="G41" t="s">
+        <v>115</v>
+      </c>
       <c r="I41">
         <v>-100</v>
       </c>
       <c r="J41" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
         <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
@@ -1750,39 +1906,42 @@
       <c r="F42" t="s">
         <v>12</v>
       </c>
+      <c r="G42" t="s">
+        <v>115</v>
+      </c>
       <c r="I42">
         <v>-100</v>
       </c>
       <c r="J42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
       </c>
       <c r="I43">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
@@ -1793,22 +1952,25 @@
       <c r="F44" t="s">
         <v>20</v>
       </c>
+      <c r="G44" t="s">
+        <v>115</v>
+      </c>
       <c r="I44">
         <v>-100</v>
       </c>
       <c r="J44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s">
         <v>10</v>
@@ -1819,22 +1981,25 @@
       <c r="F45" t="s">
         <v>20</v>
       </c>
+      <c r="G45" t="s">
+        <v>115</v>
+      </c>
       <c r="I45">
         <v>-100</v>
       </c>
       <c r="J45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -1845,212 +2010,239 @@
       <c r="F46" t="s">
         <v>20</v>
       </c>
+      <c r="G46" t="s">
+        <v>115</v>
+      </c>
       <c r="I46">
         <v>-100</v>
       </c>
       <c r="J46" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" t="s">
         <v>65</v>
       </c>
-      <c r="C47" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" t="s">
-        <v>67</v>
-      </c>
-      <c r="F47" t="s">
-        <v>68</v>
+      <c r="G47" t="s">
+        <v>115</v>
       </c>
       <c r="I47">
         <v>-100</v>
       </c>
       <c r="J47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F48" t="s">
         <v>51</v>
       </c>
+      <c r="G48" t="s">
+        <v>115</v>
+      </c>
       <c r="I48">
         <v>-100</v>
       </c>
       <c r="J48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
       </c>
+      <c r="E49" t="s">
+        <v>111</v>
+      </c>
+      <c r="F49" t="s">
+        <v>113</v>
+      </c>
       <c r="I49">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
       </c>
       <c r="I50">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" t="s">
         <v>69</v>
       </c>
-      <c r="C51" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" t="s">
-        <v>71</v>
-      </c>
-      <c r="F51" t="s">
-        <v>72</v>
+      <c r="G51" t="s">
+        <v>115</v>
       </c>
       <c r="I51">
         <v>-100</v>
       </c>
       <c r="J51" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>68</v>
+      </c>
+      <c r="F52" t="s">
         <v>69</v>
       </c>
-      <c r="C52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" t="s">
-        <v>71</v>
-      </c>
-      <c r="F52" t="s">
-        <v>72</v>
+      <c r="G52" t="s">
+        <v>115</v>
       </c>
       <c r="I52">
         <v>-100</v>
       </c>
       <c r="J52" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" t="s">
+        <v>68</v>
+      </c>
+      <c r="F53" t="s">
         <v>69</v>
       </c>
-      <c r="C53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" t="s">
-        <v>72</v>
+      <c r="G53" t="s">
+        <v>115</v>
       </c>
       <c r="I53">
         <v>-100</v>
       </c>
       <c r="J53" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>68</v>
+      </c>
+      <c r="F54" t="s">
         <v>69</v>
       </c>
-      <c r="C54" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" t="s">
-        <v>71</v>
-      </c>
-      <c r="F54" t="s">
-        <v>72</v>
+      <c r="G54" t="s">
+        <v>115</v>
       </c>
       <c r="I54">
         <v>-100</v>
       </c>
       <c r="J54" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D55" t="s">
         <v>10</v>
@@ -2061,22 +2253,25 @@
       <c r="F55" t="s">
         <v>46</v>
       </c>
+      <c r="G55" t="s">
+        <v>115</v>
+      </c>
       <c r="I55">
         <v>-100</v>
       </c>
       <c r="J55" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
@@ -2087,22 +2282,25 @@
       <c r="F56" t="s">
         <v>46</v>
       </c>
+      <c r="G56" t="s">
+        <v>115</v>
+      </c>
       <c r="I56">
         <v>-100</v>
       </c>
       <c r="J56" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
@@ -2113,22 +2311,25 @@
       <c r="F57" t="s">
         <v>17</v>
       </c>
+      <c r="G57" t="s">
+        <v>115</v>
+      </c>
       <c r="I57">
         <v>-100</v>
       </c>
       <c r="J57" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
@@ -2139,22 +2340,25 @@
       <c r="F58" t="s">
         <v>17</v>
       </c>
+      <c r="G58" t="s">
+        <v>115</v>
+      </c>
       <c r="I58">
         <v>-100</v>
       </c>
       <c r="J58" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
@@ -2165,45 +2369,51 @@
       <c r="F59" t="s">
         <v>17</v>
       </c>
+      <c r="G59" t="s">
+        <v>115</v>
+      </c>
       <c r="I59">
         <v>-100</v>
       </c>
       <c r="J59" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="F60" t="s">
         <v>46</v>
       </c>
+      <c r="G60" t="s">
+        <v>115</v>
+      </c>
       <c r="I60">
         <v>-100</v>
       </c>
       <c r="J60" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
         <v>50</v>
@@ -2211,11 +2421,17 @@
       <c r="D61" t="s">
         <v>10</v>
       </c>
+      <c r="E61" t="s">
+        <v>110</v>
+      </c>
+      <c r="F61" t="s">
+        <v>112</v>
+      </c>
+      <c r="G61" t="s">
+        <v>114</v>
+      </c>
       <c r="I61">
-        <v>-100</v>
-      </c>
-      <c r="J61" t="s">
-        <v>113</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2223,7 +2439,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
         <v>50</v>
@@ -2241,27 +2457,36 @@
         <v>52</v>
       </c>
       <c r="I62">
-        <v>57.228000000000002</v>
+        <v>84.942999999999998</v>
       </c>
       <c r="J62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D63" t="s">
         <v>10</v>
       </c>
+      <c r="E63" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" t="s">
+        <v>112</v>
+      </c>
+      <c r="G63" t="s">
+        <v>114</v>
+      </c>
       <c r="I63">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2269,10 +2494,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D64" t="s">
         <v>10</v>
@@ -2287,27 +2512,36 @@
         <v>24</v>
       </c>
       <c r="I64">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J64" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D65" t="s">
         <v>10</v>
       </c>
+      <c r="E65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65" t="s">
+        <v>112</v>
+      </c>
+      <c r="G65" t="s">
+        <v>114</v>
+      </c>
       <c r="I65">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2315,10 +2549,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D66" t="s">
         <v>10</v>
@@ -2333,27 +2567,36 @@
         <v>24</v>
       </c>
       <c r="I66">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J66" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D67" t="s">
         <v>10</v>
       </c>
+      <c r="E67" t="s">
+        <v>110</v>
+      </c>
+      <c r="F67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G67" t="s">
+        <v>114</v>
+      </c>
       <c r="I67">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -2361,28 +2604,28 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C68" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
       </c>
       <c r="E68" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F68" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G68" t="s">
         <v>24</v>
       </c>
       <c r="I68">
-        <v>85.950999999999993</v>
+        <v>90.433999999999997</v>
       </c>
       <c r="J68" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2390,28 +2633,28 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
       </c>
       <c r="E69" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F69" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G69" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I69">
-        <v>66.344999999999999</v>
+        <v>83.218000000000004</v>
       </c>
       <c r="J69" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -2419,45 +2662,54 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D70" t="s">
         <v>10</v>
       </c>
       <c r="E70" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F70" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G70" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I70">
         <v>83.218000000000004</v>
       </c>
       <c r="J70" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D71" t="s">
         <v>10</v>
       </c>
+      <c r="E71" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71" t="s">
+        <v>112</v>
+      </c>
+      <c r="G71" t="s">
+        <v>114</v>
+      </c>
       <c r="I71">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -2465,10 +2717,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C72" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
@@ -2480,30 +2732,39 @@
         <v>17</v>
       </c>
       <c r="G72" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I72">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J72" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D73" t="s">
         <v>10</v>
       </c>
+      <c r="E73" t="s">
+        <v>110</v>
+      </c>
+      <c r="F73" t="s">
+        <v>112</v>
+      </c>
+      <c r="G73" t="s">
+        <v>114</v>
+      </c>
       <c r="I73">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2511,28 +2772,28 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C74" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G74" t="s">
         <v>13</v>
       </c>
       <c r="I74">
-        <v>64.257000000000005</v>
+        <v>88.106999999999999</v>
       </c>
       <c r="J74" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2540,28 +2801,28 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
       </c>
       <c r="E75" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F75" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G75" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I75">
-        <v>72.61</v>
+        <v>90.046999999999997</v>
       </c>
       <c r="J75" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2569,45 +2830,54 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" t="s">
+        <v>82</v>
+      </c>
+      <c r="F76" t="s">
+        <v>83</v>
+      </c>
+      <c r="G76" t="s">
         <v>84</v>
-      </c>
-      <c r="C76" t="s">
-        <v>85</v>
-      </c>
-      <c r="D76" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" t="s">
-        <v>86</v>
-      </c>
-      <c r="F76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G76" t="s">
-        <v>88</v>
       </c>
       <c r="I76">
         <v>92.138000000000005</v>
       </c>
       <c r="J76" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D77" t="s">
         <v>10</v>
       </c>
+      <c r="E77" t="s">
+        <v>110</v>
+      </c>
+      <c r="F77" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" t="s">
+        <v>114</v>
+      </c>
       <c r="I77">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -2615,28 +2885,28 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D78" t="s">
         <v>10</v>
       </c>
       <c r="E78" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G78" t="s">
         <v>24</v>
       </c>
       <c r="I78">
-        <v>85.950999999999993</v>
+        <v>90.433999999999997</v>
       </c>
       <c r="J78" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2644,28 +2914,28 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C79" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D79" t="s">
         <v>10</v>
       </c>
       <c r="E79" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F79" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G79" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I79">
-        <v>66.344999999999999</v>
+        <v>83.218000000000004</v>
       </c>
       <c r="J79" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2673,45 +2943,54 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D80" t="s">
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F80" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G80" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I80">
         <v>83.218000000000004</v>
       </c>
       <c r="J80" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C81" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D81" t="s">
         <v>10</v>
       </c>
+      <c r="E81" t="s">
+        <v>110</v>
+      </c>
+      <c r="F81" t="s">
+        <v>112</v>
+      </c>
+      <c r="G81" t="s">
+        <v>114</v>
+      </c>
       <c r="I81">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -2719,10 +2998,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C82" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
@@ -2734,30 +3013,39 @@
         <v>17</v>
       </c>
       <c r="G82" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I82">
-        <v>71.415999999999997</v>
+        <v>89.043999999999997</v>
       </c>
       <c r="J82" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
       </c>
+      <c r="E83" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83" t="s">
+        <v>112</v>
+      </c>
+      <c r="G83" t="s">
+        <v>114</v>
+      </c>
       <c r="I83">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -2765,10 +3053,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C84" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
@@ -2780,13 +3068,13 @@
         <v>60</v>
       </c>
       <c r="G84" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I84">
-        <v>87.704999999999998</v>
+        <v>88.497</v>
       </c>
       <c r="J84" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -2794,10 +3082,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D85" t="s">
         <v>10</v>
@@ -2815,7 +3103,7 @@
         <v>86.384</v>
       </c>
       <c r="J85" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -2823,10 +3111,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C86" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D86" t="s">
         <v>10</v>
@@ -2838,13 +3126,13 @@
         <v>17</v>
       </c>
       <c r="G86" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I86">
-        <v>54.95</v>
+        <v>90.343999999999994</v>
       </c>
       <c r="J86" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -2852,10 +3140,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -2864,16 +3152,16 @@
         <v>27</v>
       </c>
       <c r="F87" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G87" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I87">
-        <v>89.6</v>
+        <v>91.759</v>
       </c>
       <c r="J87" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -2881,10 +3169,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -2896,47 +3184,56 @@
         <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I88">
-        <v>67.582999999999998</v>
+        <v>91.587000000000003</v>
       </c>
       <c r="J88" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
       </c>
       <c r="I89">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C90" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
       </c>
+      <c r="E90" t="s">
+        <v>110</v>
+      </c>
+      <c r="F90" t="s">
+        <v>112</v>
+      </c>
+      <c r="G90" t="s">
+        <v>114</v>
+      </c>
       <c r="I90">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -2944,10 +3241,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C91" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D91" t="s">
         <v>10</v>
@@ -2959,30 +3256,39 @@
         <v>56</v>
       </c>
       <c r="G91" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I91">
-        <v>87.662000000000006</v>
+        <v>90.75</v>
       </c>
       <c r="J91" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
       </c>
+      <c r="E92" t="s">
+        <v>110</v>
+      </c>
+      <c r="F92" t="s">
+        <v>112</v>
+      </c>
+      <c r="G92" t="s">
+        <v>114</v>
+      </c>
       <c r="I92">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -2990,10 +3296,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C93" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D93" t="s">
         <v>10</v>
@@ -3011,24 +3317,33 @@
         <v>67.394999999999996</v>
       </c>
       <c r="J93" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C94" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
       </c>
+      <c r="E94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" t="s">
+        <v>112</v>
+      </c>
+      <c r="G94" t="s">
+        <v>114</v>
+      </c>
       <c r="I94">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
@@ -3036,10 +3351,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C95" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D95" t="s">
         <v>10</v>
@@ -3051,13 +3366,13 @@
         <v>60</v>
       </c>
       <c r="G95" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I95">
-        <v>87.704999999999998</v>
+        <v>88.497</v>
       </c>
       <c r="J95" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -3065,10 +3380,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D96" t="s">
         <v>10</v>
@@ -3086,7 +3401,7 @@
         <v>86.384</v>
       </c>
       <c r="J96" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -3094,10 +3409,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D97" t="s">
         <v>10</v>
@@ -3109,13 +3424,13 @@
         <v>17</v>
       </c>
       <c r="G97" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I97">
-        <v>54.95</v>
+        <v>90.343999999999994</v>
       </c>
       <c r="J97" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -3123,10 +3438,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D98" t="s">
         <v>10</v>
@@ -3135,16 +3450,16 @@
         <v>27</v>
       </c>
       <c r="F98" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G98" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I98">
-        <v>89.6</v>
+        <v>91.759</v>
       </c>
       <c r="J98" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -3152,10 +3467,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D99" t="s">
         <v>10</v>
@@ -3167,47 +3482,56 @@
         <v>12</v>
       </c>
       <c r="G99" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I99">
-        <v>67.582999999999998</v>
+        <v>91.587000000000003</v>
       </c>
       <c r="J99" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C100" t="s">
+        <v>88</v>
+      </c>
+      <c r="D100" t="s">
+        <v>10</v>
+      </c>
+      <c r="I100">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C101" t="s">
         <v>92</v>
       </c>
-      <c r="D100" t="s">
-        <v>10</v>
-      </c>
-      <c r="I100">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>99</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C101" t="s">
-        <v>96</v>
-      </c>
       <c r="D101" t="s">
         <v>10</v>
       </c>
+      <c r="E101" t="s">
+        <v>110</v>
+      </c>
+      <c r="F101" t="s">
+        <v>112</v>
+      </c>
+      <c r="G101" t="s">
+        <v>114</v>
+      </c>
       <c r="I101">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
@@ -3215,10 +3539,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D102" t="s">
         <v>10</v>
@@ -3230,30 +3554,39 @@
         <v>56</v>
       </c>
       <c r="G102" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I102">
-        <v>87.662000000000006</v>
+        <v>90.75</v>
       </c>
       <c r="J102" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
       </c>
+      <c r="E103" t="s">
+        <v>110</v>
+      </c>
+      <c r="F103" t="s">
+        <v>112</v>
+      </c>
+      <c r="G103" t="s">
+        <v>114</v>
+      </c>
       <c r="I103">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
@@ -3261,10 +3594,10 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C104" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D104" t="s">
         <v>10</v>
@@ -3282,15 +3615,15 @@
         <v>67.394999999999996</v>
       </c>
       <c r="J104" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
@@ -3298,8 +3631,17 @@
       <c r="D105" t="s">
         <v>10</v>
       </c>
+      <c r="E105" t="s">
+        <v>110</v>
+      </c>
+      <c r="F105" t="s">
+        <v>112</v>
+      </c>
+      <c r="G105" t="s">
+        <v>114</v>
+      </c>
       <c r="I105">
-        <v>-100</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
@@ -3307,7 +3649,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
@@ -3328,7 +3670,7 @@
         <v>89.043999999999997</v>
       </c>
       <c r="J106" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -3336,7 +3678,7 @@
         <v>104</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C107" t="s">
         <v>15</v>
@@ -3354,21 +3696,21 @@
         <v>21</v>
       </c>
       <c r="I107">
-        <v>86.134</v>
+        <v>91.444000000000003</v>
       </c>
       <c r="J107" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>104</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D108" t="s">
         <v>10</v>
@@ -3377,15 +3719,15 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>104</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C109" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
@@ -3397,24 +3739,24 @@
         <v>60</v>
       </c>
       <c r="G109" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I109">
-        <v>53.613999999999997</v>
+        <v>86.093999999999994</v>
       </c>
       <c r="J109" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>104</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C110" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D110" t="s">
         <v>10</v>
@@ -3426,24 +3768,24 @@
         <v>60</v>
       </c>
       <c r="G110" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I110">
-        <v>75.444000000000003</v>
+        <v>86.093999999999994</v>
       </c>
       <c r="J110" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>104</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C111" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D111" t="s">
         <v>10</v>
@@ -3455,82 +3797,82 @@
         <v>60</v>
       </c>
       <c r="G111" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I111">
-        <v>82.494</v>
+        <v>86.087999999999994</v>
       </c>
       <c r="J111" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>104</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C112" t="s">
+        <v>101</v>
+      </c>
+      <c r="D112" t="s">
+        <v>10</v>
+      </c>
+      <c r="E112" t="s">
+        <v>68</v>
+      </c>
+      <c r="F112" t="s">
+        <v>69</v>
+      </c>
+      <c r="G112" t="s">
         <v>105</v>
       </c>
-      <c r="D112" t="s">
-        <v>10</v>
-      </c>
-      <c r="E112" t="s">
-        <v>71</v>
-      </c>
-      <c r="F112" t="s">
-        <v>72</v>
-      </c>
-      <c r="G112" t="s">
+      <c r="I112">
+        <v>84.1</v>
+      </c>
+      <c r="J112" t="s">
         <v>109</v>
       </c>
-      <c r="I112">
-        <v>63.021000000000001</v>
-      </c>
-      <c r="J112" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>104</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C113" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D113" t="s">
         <v>10</v>
       </c>
       <c r="E113" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F113" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G113" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I113">
         <v>81.691999999999993</v>
       </c>
       <c r="J113" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>104</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C114" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D114" t="s">
         <v>10</v>
@@ -3542,24 +3884,24 @@
         <v>20</v>
       </c>
       <c r="G114" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I114">
         <v>54.134</v>
       </c>
       <c r="J114" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>104</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C115" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D115" t="s">
         <v>10</v>
@@ -3571,23 +3913,23 @@
         <v>20</v>
       </c>
       <c r="G115" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I115">
         <v>86.093999999999994</v>
       </c>
       <c r="J115" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I117">
+        <f>AVERAGEIF(I2:I115,"&gt;=0")</f>
+        <v>86.620634615384603</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J115" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="x"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J115" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter>

</xml_diff>